<commit_message>
mm gas: latest memory map
</commit_message>
<xml_diff>
--- a/apps/mmGasApp/documentation/EPICS_datas.xlsx
+++ b/apps/mmGasApp/documentation/EPICS_datas.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="103">
   <si>
     <t>BARREL</t>
   </si>
@@ -252,6 +252,90 @@
   </si>
   <si>
     <t>Overpressure flow fault</t>
+  </si>
+  <si>
+    <t>Barrel warning general</t>
+  </si>
+  <si>
+    <t>Barrel fault general</t>
+  </si>
+  <si>
+    <t>Barrel flow ok (input and output flow gas is correct)</t>
+  </si>
+  <si>
+    <t>Input pressure</t>
+  </si>
+  <si>
+    <t>64.0</t>
+  </si>
+  <si>
+    <t>64.1</t>
+  </si>
+  <si>
+    <t>64.3</t>
+  </si>
+  <si>
+    <t>64.4</t>
+  </si>
+  <si>
+    <t>64.5</t>
+  </si>
+  <si>
+    <t>64.6</t>
+  </si>
+  <si>
+    <t>64.7</t>
+  </si>
+  <si>
+    <t>64.2</t>
+  </si>
+  <si>
+    <t>Input flow warning</t>
+  </si>
+  <si>
+    <t>Delta input/output flow warning</t>
+  </si>
+  <si>
+    <t>Input flow fault</t>
+  </si>
+  <si>
+    <t>Start gas command</t>
+  </si>
+  <si>
+    <t>Stop gas command</t>
+  </si>
+  <si>
+    <t>65.0</t>
+  </si>
+  <si>
+    <t>65.1</t>
+  </si>
+  <si>
+    <t>65.2</t>
+  </si>
+  <si>
+    <t>65.3</t>
+  </si>
+  <si>
+    <t>65.4</t>
+  </si>
+  <si>
+    <t>65.5</t>
+  </si>
+  <si>
+    <t>65.6</t>
+  </si>
+  <si>
+    <t>Delta input/output flow fault</t>
+  </si>
+  <si>
+    <t>65.7</t>
+  </si>
+  <si>
+    <t>Only write</t>
+  </si>
+  <si>
+    <t>empty</t>
   </si>
 </sst>
 </file>
@@ -321,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -335,6 +419,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1572,10 +1662,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1679,13 +1769,10 @@
       <c r="G5" s="2">
         <v>0</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="J5" s="6">
         <v>0</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="6" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1705,13 +1792,10 @@
       <c r="G6" s="2">
         <v>4</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="2">
+      <c r="J6" s="6">
         <v>4</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1729,13 +1813,12 @@
       <c r="G7" s="2">
         <v>8</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J7" s="2">
+      <c r="J7" s="6">
         <v>8</v>
       </c>
-      <c r="K7" s="2"/>
+      <c r="K7" s="6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1751,13 +1834,12 @@
       <c r="G8" s="2">
         <v>12</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J8" s="2">
+      <c r="J8" s="6">
         <v>12</v>
       </c>
-      <c r="K8" s="2"/>
+      <c r="K8" s="6" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -1768,11 +1850,11 @@
         <v>11</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="J9" s="2">
+      <c r="J9" s="6">
         <v>16</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>65</v>
+      <c r="K9" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1784,11 +1866,11 @@
         <v>12</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="J10" s="2">
+      <c r="J10" s="6">
         <v>20</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>66</v>
+      <c r="K10" s="6" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1800,10 +1882,12 @@
         <v>13</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="J11" s="2">
+      <c r="J11" s="6">
         <v>24</v>
       </c>
-      <c r="K11" s="2"/>
+      <c r="K11" s="6" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -1814,11 +1898,11 @@
         <v>14</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="J12" s="2">
+      <c r="J12" s="6">
         <v>28</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>67</v>
+      <c r="K12" s="6" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1826,11 +1910,11 @@
         <v>23</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="J13" s="2">
+      <c r="J13" s="6">
         <v>32</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>60</v>
+      <c r="K13" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1838,21 +1922,23 @@
         <v>24</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="J14" s="2">
+      <c r="J14" s="6">
         <v>36</v>
       </c>
-      <c r="K14" s="2"/>
+      <c r="K14" s="6" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="J15" s="2">
+      <c r="J15" s="6">
         <v>40</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>68</v>
+      <c r="K15" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1860,178 +1946,268 @@
         <v>26</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="J16" s="2">
+      <c r="J16" s="6">
         <v>44</v>
       </c>
-      <c r="K16" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="J17" s="2">
+      <c r="J17" s="6">
         <v>48</v>
       </c>
-      <c r="K17" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D18" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="J18" s="2">
+      <c r="J18" s="6">
         <v>52</v>
       </c>
-      <c r="K18" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D19" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="J19" s="2">
+      <c r="J19" s="6">
         <v>56</v>
       </c>
-      <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D20" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E20" s="2"/>
-      <c r="J20" s="2">
+      <c r="J20" s="6">
         <v>60</v>
       </c>
-      <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D21" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="2">
-        <v>64</v>
-      </c>
-      <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J21" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D22" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="2">
-        <v>68</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J22" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D23" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="2">
-        <v>72</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J23" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J24" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D25" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J25" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D26" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J26" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D27" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J27" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D28" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J28" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D29" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J29" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D30" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J30" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D31" s="2" t="s">
         <v>41</v>
       </c>
       <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J31" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D32" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="J32" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D33" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="J33" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="L33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D34" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="J34" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D35" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="J35" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D36" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E36" s="2"/>
+      <c r="J36" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>